<commit_message>
working on simaris idarecisi
</commit_message>
<xml_diff>
--- a/application/plugins/StockBuyManager/views/StockBuyOrderExport.xlsx
+++ b/application/plugins/StockBuyManager/views/StockBuyOrderExport.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="товары" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="mallar" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,28 +22,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
-    <t xml:space="preserve">Заказ поставщикам {$v-&gt;date}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Коментарий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Код</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Название</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Заказ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Потребность</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Цена</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Варианты цен поставщиков</t>
+    <t xml:space="preserve">Tedarikçige Sımarışlar {$v-&gt;date}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">İzaat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">İsim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sımarış</t>
+  </si>
+  <si>
+    <t xml:space="preserve">İhtiyaç</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiyat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tedarikçi fiyat variantları</t>
   </si>
   <si>
     <t xml:space="preserve">{$v-&gt;filter-&gt;product_comment}</t>
@@ -434,8 +434,8 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -459,7 +459,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" s="6" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>

</xml_diff>